<commit_message>
Update figs and scripts
</commit_message>
<xml_diff>
--- a/tables/Table_rhode_demulticoder_v_standardworkflow.xlsx
+++ b/tables/Table_rhode_demulticoder_v_standardworkflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudermann/benchmark_demulticoder/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B756BD1B-3C56-954C-9F2F-78F730D68EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1795B10A-A364-5648-AFF7-BCF2AF1DE71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="500" windowWidth="27640" windowHeight="16420" activeTab="1" xr2:uid="{687BCEBF-EBC6-CE4C-A1FE-79E157267389}"/>
+    <workbookView minimized="1" xWindow="1100" yWindow="500" windowWidth="27640" windowHeight="16420" activeTab="1" xr2:uid="{687BCEBF-EBC6-CE4C-A1FE-79E157267389}"/>
   </bookViews>
   <sheets>
     <sheet name="ITS" sheetId="3" r:id="rId1"/>
@@ -663,7 +663,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -725,11 +725,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -782,6 +806,42 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F36F2DE-39F3-3F4E-ACCA-874959AD90DF}">
   <dimension ref="A1:P175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K178" sqref="K178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1237,8 +1297,12 @@
         <f>M2-L2</f>
         <v>128</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="O2" s="23">
+        <v>2358</v>
+      </c>
+      <c r="P2" s="26">
+        <v>2368</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1284,8 +1348,8 @@
         <f t="shared" ref="N3:N66" si="0">M3-L3</f>
         <v>15</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="27"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1331,8 +1395,8 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="27"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1378,8 +1442,8 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="27"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1425,8 +1489,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="27"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1472,8 +1536,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="27"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -1519,8 +1583,8 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="27"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -1566,8 +1630,8 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="27"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1613,8 +1677,8 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="27"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1660,8 +1724,8 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="27"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1707,8 +1771,8 @@
         <f t="shared" si="0"/>
         <v>-37</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="27"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1754,8 +1818,8 @@
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="27"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1801,8 +1865,8 @@
         <f t="shared" si="0"/>
         <v>-317</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="27"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -1848,8 +1912,8 @@
         <f t="shared" si="0"/>
         <v>127</v>
       </c>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="27"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1895,8 +1959,8 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="27"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1942,8 +2006,8 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="27"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1989,8 +2053,8 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="27"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -2036,8 +2100,8 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="27"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -2083,8 +2147,8 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="27"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -2130,8 +2194,8 @@
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="27"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -2177,8 +2241,8 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="27"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -2224,8 +2288,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="27"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -2271,8 +2335,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="27"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -2318,8 +2382,8 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="27"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -2365,8 +2429,8 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="27"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -2412,8 +2476,8 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="27"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
@@ -2459,8 +2523,8 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="27"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -2506,8 +2570,8 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="27"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -2553,8 +2617,8 @@
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="27"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -2600,8 +2664,8 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="27"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -2647,8 +2711,8 @@
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="27"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
@@ -2694,8 +2758,8 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="27"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -2741,8 +2805,8 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="27"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -2788,8 +2852,8 @@
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="27"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -2835,8 +2899,8 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="27"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -2882,8 +2946,8 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="27"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -2929,8 +2993,8 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="27"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
@@ -2976,8 +3040,8 @@
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="27"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
@@ -3023,8 +3087,8 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="27"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -3070,8 +3134,8 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="27"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
@@ -3117,8 +3181,8 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="27"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
@@ -3164,8 +3228,8 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="27"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
@@ -3211,8 +3275,8 @@
         <f t="shared" si="0"/>
         <v>-190</v>
       </c>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="27"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
@@ -3258,8 +3322,8 @@
         <f t="shared" si="0"/>
         <v>147</v>
       </c>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="27"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
@@ -3305,8 +3369,8 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="27"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
@@ -3352,8 +3416,8 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
+      <c r="O47" s="24"/>
+      <c r="P47" s="27"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
@@ -3399,8 +3463,8 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
+      <c r="O48" s="24"/>
+      <c r="P48" s="27"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
@@ -3446,8 +3510,8 @@
         <f t="shared" si="0"/>
         <v>141</v>
       </c>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="27"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
@@ -3493,8 +3557,8 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
+      <c r="O50" s="24"/>
+      <c r="P50" s="27"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
@@ -3540,8 +3604,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="27"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
@@ -3587,8 +3651,8 @@
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
+      <c r="O52" s="24"/>
+      <c r="P52" s="27"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
@@ -3634,8 +3698,8 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
+      <c r="O53" s="24"/>
+      <c r="P53" s="27"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
@@ -3681,8 +3745,8 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="27"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
@@ -3728,8 +3792,8 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="27"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
@@ -3775,8 +3839,8 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
+      <c r="O56" s="24"/>
+      <c r="P56" s="27"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -3822,8 +3886,8 @@
         <f t="shared" si="0"/>
         <v>167</v>
       </c>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
+      <c r="O57" s="24"/>
+      <c r="P57" s="27"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
@@ -3869,8 +3933,8 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
+      <c r="O58" s="24"/>
+      <c r="P58" s="27"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
@@ -3916,8 +3980,8 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
+      <c r="O59" s="24"/>
+      <c r="P59" s="27"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
@@ -3963,8 +4027,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
+      <c r="O60" s="24"/>
+      <c r="P60" s="27"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
@@ -4010,8 +4074,8 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
+      <c r="O61" s="24"/>
+      <c r="P61" s="27"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
@@ -4057,8 +4121,8 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
+      <c r="O62" s="24"/>
+      <c r="P62" s="27"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
@@ -4104,8 +4168,8 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
+      <c r="O63" s="24"/>
+      <c r="P63" s="27"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
@@ -4151,8 +4215,8 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
+      <c r="O64" s="24"/>
+      <c r="P64" s="27"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
@@ -4198,8 +4262,8 @@
         <f t="shared" si="0"/>
         <v>276</v>
       </c>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
+      <c r="O65" s="24"/>
+      <c r="P65" s="27"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
@@ -4245,8 +4309,8 @@
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
+      <c r="O66" s="24"/>
+      <c r="P66" s="27"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
@@ -4292,8 +4356,8 @@
         <f t="shared" ref="N67:N130" si="1">M67-L67</f>
         <v>73</v>
       </c>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
+      <c r="O67" s="24"/>
+      <c r="P67" s="27"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
@@ -4339,8 +4403,8 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
+      <c r="O68" s="24"/>
+      <c r="P68" s="27"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -4386,8 +4450,8 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="O69" s="4"/>
-      <c r="P69" s="4"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="27"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
@@ -4433,8 +4497,8 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="O70" s="4"/>
-      <c r="P70" s="4"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="27"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
@@ -4480,8 +4544,8 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
+      <c r="O71" s="24"/>
+      <c r="P71" s="27"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
@@ -4527,8 +4591,8 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="O72" s="4"/>
-      <c r="P72" s="4"/>
+      <c r="O72" s="24"/>
+      <c r="P72" s="27"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
@@ -4574,8 +4638,8 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="O73" s="4"/>
-      <c r="P73" s="4"/>
+      <c r="O73" s="24"/>
+      <c r="P73" s="27"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
@@ -4621,8 +4685,8 @@
         <f t="shared" si="1"/>
         <v>-185</v>
       </c>
-      <c r="O74" s="4"/>
-      <c r="P74" s="4"/>
+      <c r="O74" s="24"/>
+      <c r="P74" s="27"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
@@ -4668,8 +4732,8 @@
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
+      <c r="O75" s="24"/>
+      <c r="P75" s="27"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
@@ -4715,8 +4779,8 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
+      <c r="O76" s="24"/>
+      <c r="P76" s="27"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
@@ -4762,8 +4826,8 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
+      <c r="O77" s="24"/>
+      <c r="P77" s="27"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
@@ -4809,8 +4873,8 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
+      <c r="O78" s="24"/>
+      <c r="P78" s="27"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
@@ -4856,8 +4920,8 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
+      <c r="O79" s="24"/>
+      <c r="P79" s="27"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
@@ -4903,8 +4967,8 @@
         <f t="shared" si="1"/>
         <v>-216</v>
       </c>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
+      <c r="O80" s="24"/>
+      <c r="P80" s="27"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
@@ -4950,8 +5014,8 @@
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
+      <c r="O81" s="24"/>
+      <c r="P81" s="27"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
@@ -4997,8 +5061,8 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
+      <c r="O82" s="24"/>
+      <c r="P82" s="27"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
@@ -5044,8 +5108,8 @@
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
+      <c r="O83" s="24"/>
+      <c r="P83" s="27"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
@@ -5091,8 +5155,8 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
+      <c r="O84" s="24"/>
+      <c r="P84" s="27"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
@@ -5138,8 +5202,8 @@
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
+      <c r="O85" s="24"/>
+      <c r="P85" s="27"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
@@ -5185,8 +5249,8 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
+      <c r="O86" s="24"/>
+      <c r="P86" s="27"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
@@ -5232,8 +5296,8 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
+      <c r="O87" s="24"/>
+      <c r="P87" s="27"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
@@ -5279,8 +5343,8 @@
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
-      <c r="O88" s="4"/>
-      <c r="P88" s="4"/>
+      <c r="O88" s="24"/>
+      <c r="P88" s="27"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
@@ -5326,8 +5390,8 @@
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="O89" s="4"/>
-      <c r="P89" s="4"/>
+      <c r="O89" s="24"/>
+      <c r="P89" s="27"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
@@ -5373,8 +5437,8 @@
         <f t="shared" si="1"/>
         <v>164</v>
       </c>
-      <c r="O90" s="4"/>
-      <c r="P90" s="4"/>
+      <c r="O90" s="24"/>
+      <c r="P90" s="27"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
@@ -5420,8 +5484,8 @@
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
+      <c r="O91" s="24"/>
+      <c r="P91" s="27"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
@@ -5467,8 +5531,8 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
+      <c r="O92" s="24"/>
+      <c r="P92" s="27"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
@@ -5514,8 +5578,8 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="O93" s="4"/>
-      <c r="P93" s="4"/>
+      <c r="O93" s="24"/>
+      <c r="P93" s="27"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
@@ -5561,8 +5625,8 @@
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="O94" s="4"/>
-      <c r="P94" s="4"/>
+      <c r="O94" s="24"/>
+      <c r="P94" s="27"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
@@ -5608,8 +5672,8 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="O95" s="4"/>
-      <c r="P95" s="4"/>
+      <c r="O95" s="24"/>
+      <c r="P95" s="27"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
@@ -5655,8 +5719,8 @@
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="O96" s="4"/>
-      <c r="P96" s="4"/>
+      <c r="O96" s="24"/>
+      <c r="P96" s="27"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
@@ -5702,8 +5766,8 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="O97" s="4"/>
-      <c r="P97" s="4"/>
+      <c r="O97" s="24"/>
+      <c r="P97" s="27"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
@@ -5749,8 +5813,8 @@
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
-      <c r="O98" s="4"/>
-      <c r="P98" s="4"/>
+      <c r="O98" s="24"/>
+      <c r="P98" s="27"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
@@ -5796,8 +5860,8 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
+      <c r="O99" s="24"/>
+      <c r="P99" s="27"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
@@ -5843,8 +5907,8 @@
         <f t="shared" si="1"/>
         <v>292</v>
       </c>
-      <c r="O100" s="4"/>
-      <c r="P100" s="4"/>
+      <c r="O100" s="24"/>
+      <c r="P100" s="27"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
@@ -5890,8 +5954,8 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
+      <c r="O101" s="24"/>
+      <c r="P101" s="27"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
@@ -5937,8 +6001,8 @@
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
+      <c r="O102" s="24"/>
+      <c r="P102" s="27"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
@@ -5984,8 +6048,8 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
+      <c r="O103" s="24"/>
+      <c r="P103" s="27"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
@@ -6031,8 +6095,8 @@
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
-      <c r="O104" s="4"/>
-      <c r="P104" s="4"/>
+      <c r="O104" s="24"/>
+      <c r="P104" s="27"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
@@ -6078,8 +6142,8 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
+      <c r="O105" s="24"/>
+      <c r="P105" s="27"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
@@ -6125,8 +6189,8 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="O106" s="4"/>
-      <c r="P106" s="4"/>
+      <c r="O106" s="24"/>
+      <c r="P106" s="27"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
@@ -6172,8 +6236,8 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="O107" s="4"/>
-      <c r="P107" s="4"/>
+      <c r="O107" s="24"/>
+      <c r="P107" s="27"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
@@ -6219,8 +6283,8 @@
         <f t="shared" si="1"/>
         <v>159</v>
       </c>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
+      <c r="O108" s="24"/>
+      <c r="P108" s="27"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
@@ -6266,8 +6330,8 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O109" s="4"/>
-      <c r="P109" s="4"/>
+      <c r="O109" s="24"/>
+      <c r="P109" s="27"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
@@ -6313,8 +6377,8 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="O110" s="4"/>
-      <c r="P110" s="4"/>
+      <c r="O110" s="24"/>
+      <c r="P110" s="27"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
@@ -6360,8 +6424,8 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="O111" s="4"/>
-      <c r="P111" s="4"/>
+      <c r="O111" s="24"/>
+      <c r="P111" s="27"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
@@ -6407,8 +6471,8 @@
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
+      <c r="O112" s="24"/>
+      <c r="P112" s="27"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
@@ -6454,8 +6518,8 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
+      <c r="O113" s="24"/>
+      <c r="P113" s="27"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
@@ -6501,8 +6565,8 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
+      <c r="O114" s="24"/>
+      <c r="P114" s="27"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
@@ -6548,8 +6612,8 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="O115" s="4"/>
-      <c r="P115" s="4"/>
+      <c r="O115" s="24"/>
+      <c r="P115" s="27"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
@@ -6595,8 +6659,8 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="O116" s="4"/>
-      <c r="P116" s="4"/>
+      <c r="O116" s="24"/>
+      <c r="P116" s="27"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
@@ -6642,8 +6706,8 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
+      <c r="O117" s="24"/>
+      <c r="P117" s="27"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
@@ -6689,8 +6753,8 @@
         <f t="shared" si="1"/>
         <v>-137</v>
       </c>
-      <c r="O118" s="4"/>
-      <c r="P118" s="4"/>
+      <c r="O118" s="24"/>
+      <c r="P118" s="27"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
@@ -6736,8 +6800,8 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="O119" s="4"/>
-      <c r="P119" s="4"/>
+      <c r="O119" s="24"/>
+      <c r="P119" s="27"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
@@ -6783,8 +6847,8 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
+      <c r="O120" s="24"/>
+      <c r="P120" s="27"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
@@ -6830,8 +6894,8 @@
         <f t="shared" si="1"/>
         <v>368</v>
       </c>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
+      <c r="O121" s="24"/>
+      <c r="P121" s="27"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
@@ -6877,8 +6941,8 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
+      <c r="O122" s="24"/>
+      <c r="P122" s="27"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
@@ -6924,8 +6988,8 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="O123" s="4"/>
-      <c r="P123" s="4"/>
+      <c r="O123" s="24"/>
+      <c r="P123" s="27"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
@@ -6971,8 +7035,8 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="O124" s="4"/>
-      <c r="P124" s="4"/>
+      <c r="O124" s="24"/>
+      <c r="P124" s="27"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
@@ -7018,8 +7082,8 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="O125" s="4"/>
-      <c r="P125" s="4"/>
+      <c r="O125" s="24"/>
+      <c r="P125" s="27"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
@@ -7065,8 +7129,8 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
+      <c r="O126" s="24"/>
+      <c r="P126" s="27"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
@@ -7112,8 +7176,8 @@
         <f t="shared" si="1"/>
         <v>-170</v>
       </c>
-      <c r="O127" s="4"/>
-      <c r="P127" s="4"/>
+      <c r="O127" s="24"/>
+      <c r="P127" s="27"/>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
@@ -7159,8 +7223,8 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="O128" s="4"/>
-      <c r="P128" s="4"/>
+      <c r="O128" s="24"/>
+      <c r="P128" s="27"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
@@ -7206,8 +7270,8 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="O129" s="4"/>
-      <c r="P129" s="4"/>
+      <c r="O129" s="24"/>
+      <c r="P129" s="27"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
@@ -7253,8 +7317,8 @@
         <f t="shared" si="1"/>
         <v>619</v>
       </c>
-      <c r="O130" s="4"/>
-      <c r="P130" s="4"/>
+      <c r="O130" s="24"/>
+      <c r="P130" s="27"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
@@ -7300,8 +7364,8 @@
         <f t="shared" ref="N131:N175" si="2">M131-L131</f>
         <v>137</v>
       </c>
-      <c r="O131" s="4"/>
-      <c r="P131" s="4"/>
+      <c r="O131" s="24"/>
+      <c r="P131" s="27"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
@@ -7347,8 +7411,8 @@
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="O132" s="4"/>
-      <c r="P132" s="4"/>
+      <c r="O132" s="24"/>
+      <c r="P132" s="27"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
@@ -7394,8 +7458,8 @@
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
-      <c r="O133" s="4"/>
-      <c r="P133" s="4"/>
+      <c r="O133" s="24"/>
+      <c r="P133" s="27"/>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
@@ -7441,8 +7505,8 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="O134" s="4"/>
-      <c r="P134" s="4"/>
+      <c r="O134" s="24"/>
+      <c r="P134" s="27"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
@@ -7488,8 +7552,8 @@
         <f t="shared" si="2"/>
         <v>-98</v>
       </c>
-      <c r="O135" s="4"/>
-      <c r="P135" s="4"/>
+      <c r="O135" s="24"/>
+      <c r="P135" s="27"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
@@ -7535,8 +7599,8 @@
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="O136" s="4"/>
-      <c r="P136" s="4"/>
+      <c r="O136" s="24"/>
+      <c r="P136" s="27"/>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
@@ -7582,8 +7646,8 @@
         <f t="shared" si="2"/>
         <v>-228</v>
       </c>
-      <c r="O137" s="4"/>
-      <c r="P137" s="4"/>
+      <c r="O137" s="24"/>
+      <c r="P137" s="27"/>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
@@ -7629,8 +7693,8 @@
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="O138" s="4"/>
-      <c r="P138" s="4"/>
+      <c r="O138" s="24"/>
+      <c r="P138" s="27"/>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
@@ -7676,8 +7740,8 @@
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
+      <c r="O139" s="24"/>
+      <c r="P139" s="27"/>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
@@ -7723,8 +7787,8 @@
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
+      <c r="O140" s="24"/>
+      <c r="P140" s="27"/>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
@@ -7770,8 +7834,8 @@
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="O141" s="4"/>
-      <c r="P141" s="4"/>
+      <c r="O141" s="24"/>
+      <c r="P141" s="27"/>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
@@ -7817,8 +7881,8 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="O142" s="4"/>
-      <c r="P142" s="4"/>
+      <c r="O142" s="24"/>
+      <c r="P142" s="27"/>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
@@ -7864,8 +7928,8 @@
         <f t="shared" si="2"/>
         <v>-41</v>
       </c>
-      <c r="O143" s="4"/>
-      <c r="P143" s="4"/>
+      <c r="O143" s="24"/>
+      <c r="P143" s="27"/>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
@@ -7911,8 +7975,8 @@
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="O144" s="4"/>
-      <c r="P144" s="4"/>
+      <c r="O144" s="24"/>
+      <c r="P144" s="27"/>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
@@ -7958,8 +8022,8 @@
         <f t="shared" si="2"/>
         <v>546</v>
       </c>
-      <c r="O145" s="4"/>
-      <c r="P145" s="4"/>
+      <c r="O145" s="24"/>
+      <c r="P145" s="27"/>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
@@ -8005,8 +8069,8 @@
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
-      <c r="O146" s="4"/>
-      <c r="P146" s="4"/>
+      <c r="O146" s="24"/>
+      <c r="P146" s="27"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
@@ -8052,8 +8116,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O147" s="4"/>
-      <c r="P147" s="4"/>
+      <c r="O147" s="24"/>
+      <c r="P147" s="27"/>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
@@ -8099,8 +8163,8 @@
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
-      <c r="O148" s="4"/>
-      <c r="P148" s="4"/>
+      <c r="O148" s="24"/>
+      <c r="P148" s="27"/>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
@@ -8146,8 +8210,8 @@
         <f t="shared" si="2"/>
         <v>238</v>
       </c>
-      <c r="O149" s="4"/>
-      <c r="P149" s="4"/>
+      <c r="O149" s="24"/>
+      <c r="P149" s="27"/>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
@@ -8193,8 +8257,8 @@
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="O150" s="4"/>
-      <c r="P150" s="4"/>
+      <c r="O150" s="24"/>
+      <c r="P150" s="27"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
@@ -8240,8 +8304,8 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="O151" s="4"/>
-      <c r="P151" s="4"/>
+      <c r="O151" s="24"/>
+      <c r="P151" s="27"/>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
@@ -8287,8 +8351,8 @@
         <f t="shared" si="2"/>
         <v>202</v>
       </c>
-      <c r="O152" s="4"/>
-      <c r="P152" s="4"/>
+      <c r="O152" s="24"/>
+      <c r="P152" s="27"/>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
@@ -8334,8 +8398,8 @@
         <f t="shared" si="2"/>
         <v>275</v>
       </c>
-      <c r="O153" s="4"/>
-      <c r="P153" s="4"/>
+      <c r="O153" s="24"/>
+      <c r="P153" s="27"/>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
@@ -8381,8 +8445,8 @@
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
-      <c r="O154" s="4"/>
-      <c r="P154" s="4"/>
+      <c r="O154" s="24"/>
+      <c r="P154" s="27"/>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
@@ -8428,8 +8492,8 @@
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="O155" s="4"/>
-      <c r="P155" s="4"/>
+      <c r="O155" s="24"/>
+      <c r="P155" s="27"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
@@ -8475,8 +8539,8 @@
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="O156" s="4"/>
-      <c r="P156" s="4"/>
+      <c r="O156" s="24"/>
+      <c r="P156" s="27"/>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
@@ -8522,8 +8586,8 @@
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="O157" s="4"/>
-      <c r="P157" s="4"/>
+      <c r="O157" s="24"/>
+      <c r="P157" s="27"/>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
@@ -8569,8 +8633,8 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="O158" s="4"/>
-      <c r="P158" s="4"/>
+      <c r="O158" s="24"/>
+      <c r="P158" s="27"/>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
@@ -8616,8 +8680,8 @@
         <f t="shared" si="2"/>
         <v>117</v>
       </c>
-      <c r="O159" s="4"/>
-      <c r="P159" s="4"/>
+      <c r="O159" s="24"/>
+      <c r="P159" s="27"/>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
@@ -8663,8 +8727,8 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="O160" s="4"/>
-      <c r="P160" s="4"/>
+      <c r="O160" s="24"/>
+      <c r="P160" s="27"/>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
@@ -8710,8 +8774,8 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="O161" s="4"/>
-      <c r="P161" s="4"/>
+      <c r="O161" s="24"/>
+      <c r="P161" s="27"/>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
@@ -8757,8 +8821,8 @@
         <f t="shared" si="2"/>
         <v>113</v>
       </c>
-      <c r="O162" s="4"/>
-      <c r="P162" s="4"/>
+      <c r="O162" s="24"/>
+      <c r="P162" s="27"/>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
@@ -8804,8 +8868,8 @@
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="O163" s="4"/>
-      <c r="P163" s="4"/>
+      <c r="O163" s="24"/>
+      <c r="P163" s="27"/>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
@@ -8851,8 +8915,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O164" s="4"/>
-      <c r="P164" s="4"/>
+      <c r="O164" s="24"/>
+      <c r="P164" s="27"/>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
@@ -8898,8 +8962,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O165" s="4"/>
-      <c r="P165" s="4"/>
+      <c r="O165" s="24"/>
+      <c r="P165" s="27"/>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
@@ -8945,8 +9009,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O166" s="4"/>
-      <c r="P166" s="4"/>
+      <c r="O166" s="24"/>
+      <c r="P166" s="27"/>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
@@ -8992,8 +9056,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O167" s="4"/>
-      <c r="P167" s="4"/>
+      <c r="O167" s="24"/>
+      <c r="P167" s="27"/>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
@@ -9039,8 +9103,8 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="O168" s="4"/>
-      <c r="P168" s="4"/>
+      <c r="O168" s="24"/>
+      <c r="P168" s="27"/>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
@@ -9086,8 +9150,8 @@
         <f t="shared" si="2"/>
         <v>-13</v>
       </c>
-      <c r="O169" s="4"/>
-      <c r="P169" s="4"/>
+      <c r="O169" s="24"/>
+      <c r="P169" s="27"/>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
@@ -9133,8 +9197,8 @@
         <f t="shared" si="2"/>
         <v>331</v>
       </c>
-      <c r="O170" s="4"/>
-      <c r="P170" s="4"/>
+      <c r="O170" s="24"/>
+      <c r="P170" s="27"/>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
@@ -9180,8 +9244,8 @@
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="O171" s="4"/>
-      <c r="P171" s="4"/>
+      <c r="O171" s="24"/>
+      <c r="P171" s="27"/>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
@@ -9227,8 +9291,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O172" s="4"/>
-      <c r="P172" s="4"/>
+      <c r="O172" s="24"/>
+      <c r="P172" s="27"/>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
@@ -9274,8 +9338,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O173" s="4"/>
-      <c r="P173" s="4"/>
+      <c r="O173" s="24"/>
+      <c r="P173" s="27"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
@@ -9321,8 +9385,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O174" s="4"/>
-      <c r="P174" s="4"/>
+      <c r="O174" s="24"/>
+      <c r="P174" s="27"/>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
@@ -9367,10 +9431,14 @@
       <c r="N175" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="O175" s="4"/>
-      <c r="P175" s="4"/>
+      <c r="O175" s="25"/>
+      <c r="P175" s="28"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="P2:P175"/>
+    <mergeCell ref="O2:O175"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9379,8 +9447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C9FB8B-4AD3-E64A-B373-CD1B422F878D}">
   <dimension ref="A1:P175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P96" sqref="P96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9490,8 +9558,12 @@
         <f>M2-L2</f>
         <v>37</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="O2" s="29">
+        <v>347</v>
+      </c>
+      <c r="P2" s="20">
+        <v>347</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -9537,8 +9609,8 @@
         <f t="shared" ref="N3:N66" si="0">M3-L3</f>
         <v>19</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -9584,8 +9656,8 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -9631,8 +9703,8 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="21"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
@@ -9678,8 +9750,8 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="21"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
@@ -9725,8 +9797,8 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="21"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -9772,8 +9844,8 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
@@ -9819,8 +9891,8 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="21"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
@@ -9866,8 +9938,8 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="21"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
@@ -9913,8 +9985,8 @@
         <f t="shared" si="0"/>
         <v>171</v>
       </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
@@ -9960,8 +10032,8 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="21"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
@@ -10007,8 +10079,8 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="21"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
@@ -10054,8 +10126,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="21"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -10101,8 +10173,8 @@
         <f t="shared" si="0"/>
         <v>143</v>
       </c>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="21"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
@@ -10148,8 +10220,8 @@
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="21"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
@@ -10195,8 +10267,8 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="21"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
@@ -10242,8 +10314,8 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="21"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
@@ -10289,8 +10361,8 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="21"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
@@ -10336,8 +10408,8 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="21"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
@@ -10383,8 +10455,8 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="21"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
@@ -10430,8 +10502,8 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="21"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
@@ -10477,8 +10549,8 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="21"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
@@ -10524,8 +10596,8 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="21"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
@@ -10571,8 +10643,8 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="21"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
@@ -10618,8 +10690,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="21"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
@@ -10665,8 +10737,8 @@
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="21"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
@@ -10712,8 +10784,8 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="21"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
@@ -10759,8 +10831,8 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="21"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
@@ -10806,8 +10878,8 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="21"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
@@ -10853,8 +10925,8 @@
         <f t="shared" si="0"/>
         <v>133</v>
       </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="21"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
@@ -10900,8 +10972,8 @@
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="21"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
@@ -10947,8 +11019,8 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="21"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
@@ -10994,8 +11066,8 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="21"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
@@ -11041,8 +11113,8 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="21"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
@@ -11088,8 +11160,8 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="21"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
@@ -11135,8 +11207,8 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
+      <c r="O37" s="30"/>
+      <c r="P37" s="21"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
@@ -11182,8 +11254,8 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="21"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
@@ -11229,8 +11301,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="21"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
@@ -11276,8 +11348,8 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="21"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
@@ -11323,8 +11395,8 @@
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="21"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
@@ -11370,8 +11442,8 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
+      <c r="O42" s="30"/>
+      <c r="P42" s="21"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
@@ -11417,8 +11489,8 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
+      <c r="O43" s="30"/>
+      <c r="P43" s="21"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -11464,8 +11536,8 @@
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
+      <c r="O44" s="30"/>
+      <c r="P44" s="21"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
@@ -11511,8 +11583,8 @@
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
+      <c r="O45" s="30"/>
+      <c r="P45" s="21"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
@@ -11558,8 +11630,8 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
+      <c r="O46" s="30"/>
+      <c r="P46" s="21"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
@@ -11605,8 +11677,8 @@
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
+      <c r="O47" s="30"/>
+      <c r="P47" s="21"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
@@ -11652,8 +11724,8 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
+      <c r="O48" s="30"/>
+      <c r="P48" s="21"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
@@ -11699,8 +11771,8 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
+      <c r="O49" s="30"/>
+      <c r="P49" s="21"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
@@ -11746,8 +11818,8 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
+      <c r="O50" s="30"/>
+      <c r="P50" s="21"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
@@ -11793,8 +11865,8 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="21"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
@@ -11840,8 +11912,8 @@
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
+      <c r="O52" s="30"/>
+      <c r="P52" s="21"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
@@ -11887,8 +11959,8 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
+      <c r="O53" s="30"/>
+      <c r="P53" s="21"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
@@ -11934,8 +12006,8 @@
         <f t="shared" si="0"/>
         <v>131</v>
       </c>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
+      <c r="O54" s="30"/>
+      <c r="P54" s="21"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
@@ -11981,8 +12053,8 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
+      <c r="O55" s="30"/>
+      <c r="P55" s="21"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
@@ -12028,8 +12100,8 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
+      <c r="O56" s="30"/>
+      <c r="P56" s="21"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
@@ -12075,8 +12147,8 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
+      <c r="O57" s="30"/>
+      <c r="P57" s="21"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
@@ -12122,8 +12194,8 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
+      <c r="O58" s="30"/>
+      <c r="P58" s="21"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
@@ -12169,8 +12241,8 @@
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
+      <c r="O59" s="30"/>
+      <c r="P59" s="21"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
@@ -12216,8 +12288,8 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
+      <c r="O60" s="30"/>
+      <c r="P60" s="21"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
@@ -12263,8 +12335,8 @@
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
+      <c r="O61" s="30"/>
+      <c r="P61" s="21"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
@@ -12310,8 +12382,8 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
+      <c r="O62" s="30"/>
+      <c r="P62" s="21"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
@@ -12357,8 +12429,8 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
+      <c r="O63" s="30"/>
+      <c r="P63" s="21"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
@@ -12404,8 +12476,8 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
+      <c r="O64" s="30"/>
+      <c r="P64" s="21"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
@@ -12451,8 +12523,8 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
+      <c r="O65" s="30"/>
+      <c r="P65" s="21"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
@@ -12498,8 +12570,8 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
+      <c r="O66" s="30"/>
+      <c r="P66" s="21"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
@@ -12545,8 +12617,8 @@
         <f t="shared" ref="N67:N130" si="1">M67-L67</f>
         <v>49</v>
       </c>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
+      <c r="O67" s="30"/>
+      <c r="P67" s="21"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
@@ -12592,8 +12664,8 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
+      <c r="O68" s="30"/>
+      <c r="P68" s="21"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
@@ -12639,8 +12711,8 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="O69" s="4"/>
-      <c r="P69" s="4"/>
+      <c r="O69" s="30"/>
+      <c r="P69" s="21"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
@@ -12686,8 +12758,8 @@
         <f t="shared" si="1"/>
         <v>-255</v>
       </c>
-      <c r="O70" s="4"/>
-      <c r="P70" s="4"/>
+      <c r="O70" s="30"/>
+      <c r="P70" s="21"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
@@ -12733,8 +12805,8 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
+      <c r="O71" s="30"/>
+      <c r="P71" s="21"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
@@ -12780,8 +12852,8 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="O72" s="4"/>
-      <c r="P72" s="4"/>
+      <c r="O72" s="30"/>
+      <c r="P72" s="21"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
@@ -12827,8 +12899,8 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="O73" s="4"/>
-      <c r="P73" s="4"/>
+      <c r="O73" s="30"/>
+      <c r="P73" s="21"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
@@ -12874,8 +12946,8 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="O74" s="4"/>
-      <c r="P74" s="4"/>
+      <c r="O74" s="30"/>
+      <c r="P74" s="21"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
@@ -12921,8 +12993,8 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
+      <c r="O75" s="30"/>
+      <c r="P75" s="21"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
@@ -12968,8 +13040,8 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
+      <c r="O76" s="30"/>
+      <c r="P76" s="21"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
@@ -13015,8 +13087,8 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
+      <c r="O77" s="30"/>
+      <c r="P77" s="21"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
@@ -13062,8 +13134,8 @@
         <f t="shared" si="1"/>
         <v>212</v>
       </c>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
+      <c r="O78" s="30"/>
+      <c r="P78" s="21"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
@@ -13109,8 +13181,8 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
+      <c r="O79" s="30"/>
+      <c r="P79" s="21"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
@@ -13156,8 +13228,8 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
+      <c r="O80" s="30"/>
+      <c r="P80" s="21"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
@@ -13203,8 +13275,8 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
+      <c r="O81" s="30"/>
+      <c r="P81" s="21"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
@@ -13250,8 +13322,8 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
+      <c r="O82" s="30"/>
+      <c r="P82" s="21"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
@@ -13297,8 +13369,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
+      <c r="O83" s="30"/>
+      <c r="P83" s="21"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
@@ -13344,8 +13416,8 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
+      <c r="O84" s="30"/>
+      <c r="P84" s="21"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
@@ -13391,8 +13463,8 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
+      <c r="O85" s="30"/>
+      <c r="P85" s="21"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
@@ -13438,8 +13510,8 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
+      <c r="O86" s="30"/>
+      <c r="P86" s="21"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
@@ -13485,8 +13557,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
+      <c r="O87" s="30"/>
+      <c r="P87" s="21"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
@@ -13532,8 +13604,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O88" s="4"/>
-      <c r="P88" s="4"/>
+      <c r="O88" s="30"/>
+      <c r="P88" s="21"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
@@ -13579,8 +13651,8 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="O89" s="4"/>
-      <c r="P89" s="4"/>
+      <c r="O89" s="30"/>
+      <c r="P89" s="21"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
@@ -13626,8 +13698,8 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O90" s="4"/>
-      <c r="P90" s="4"/>
+      <c r="O90" s="30"/>
+      <c r="P90" s="21"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
@@ -13673,8 +13745,8 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
+      <c r="O91" s="30"/>
+      <c r="P91" s="21"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
@@ -13720,8 +13792,8 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
+      <c r="O92" s="30"/>
+      <c r="P92" s="21"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
@@ -13767,8 +13839,8 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O93" s="4"/>
-      <c r="P93" s="4"/>
+      <c r="O93" s="30"/>
+      <c r="P93" s="21"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
@@ -13814,8 +13886,8 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="O94" s="4"/>
-      <c r="P94" s="4"/>
+      <c r="O94" s="30"/>
+      <c r="P94" s="21"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
@@ -13861,8 +13933,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O95" s="4"/>
-      <c r="P95" s="4"/>
+      <c r="O95" s="30"/>
+      <c r="P95" s="21"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
@@ -13908,8 +13980,8 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="O96" s="4"/>
-      <c r="P96" s="4"/>
+      <c r="O96" s="30"/>
+      <c r="P96" s="21"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
@@ -13955,8 +14027,8 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="O97" s="4"/>
-      <c r="P97" s="4"/>
+      <c r="O97" s="30"/>
+      <c r="P97" s="21"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
@@ -14002,8 +14074,8 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="O98" s="4"/>
-      <c r="P98" s="4"/>
+      <c r="O98" s="30"/>
+      <c r="P98" s="21"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
@@ -14049,8 +14121,8 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
+      <c r="O99" s="30"/>
+      <c r="P99" s="21"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
@@ -14096,8 +14168,8 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="O100" s="4"/>
-      <c r="P100" s="4"/>
+      <c r="O100" s="30"/>
+      <c r="P100" s="21"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
@@ -14143,8 +14215,8 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
+      <c r="O101" s="30"/>
+      <c r="P101" s="21"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
@@ -14190,8 +14262,8 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
+      <c r="O102" s="30"/>
+      <c r="P102" s="21"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
@@ -14237,8 +14309,8 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
+      <c r="O103" s="30"/>
+      <c r="P103" s="21"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
@@ -14284,8 +14356,8 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="O104" s="4"/>
-      <c r="P104" s="4"/>
+      <c r="O104" s="30"/>
+      <c r="P104" s="21"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
@@ -14331,8 +14403,8 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
+      <c r="O105" s="30"/>
+      <c r="P105" s="21"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
@@ -14378,8 +14450,8 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="O106" s="4"/>
-      <c r="P106" s="4"/>
+      <c r="O106" s="30"/>
+      <c r="P106" s="21"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
@@ -14425,8 +14497,8 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="O107" s="4"/>
-      <c r="P107" s="4"/>
+      <c r="O107" s="30"/>
+      <c r="P107" s="21"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
@@ -14472,8 +14544,8 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
+      <c r="O108" s="30"/>
+      <c r="P108" s="21"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
@@ -14519,8 +14591,8 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="O109" s="4"/>
-      <c r="P109" s="4"/>
+      <c r="O109" s="30"/>
+      <c r="P109" s="21"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
@@ -14566,8 +14638,8 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="O110" s="4"/>
-      <c r="P110" s="4"/>
+      <c r="O110" s="30"/>
+      <c r="P110" s="21"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
@@ -14613,8 +14685,8 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="O111" s="4"/>
-      <c r="P111" s="4"/>
+      <c r="O111" s="30"/>
+      <c r="P111" s="21"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
@@ -14660,8 +14732,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
+      <c r="O112" s="30"/>
+      <c r="P112" s="21"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
@@ -14707,8 +14779,8 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
+      <c r="O113" s="30"/>
+      <c r="P113" s="21"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
@@ -14754,8 +14826,8 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
+      <c r="O114" s="30"/>
+      <c r="P114" s="21"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
@@ -14801,8 +14873,8 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="O115" s="4"/>
-      <c r="P115" s="4"/>
+      <c r="O115" s="30"/>
+      <c r="P115" s="21"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
@@ -14848,8 +14920,8 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="O116" s="4"/>
-      <c r="P116" s="4"/>
+      <c r="O116" s="30"/>
+      <c r="P116" s="21"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
@@ -14895,8 +14967,8 @@
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
+      <c r="O117" s="30"/>
+      <c r="P117" s="21"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
@@ -14942,8 +15014,8 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="O118" s="4"/>
-      <c r="P118" s="4"/>
+      <c r="O118" s="30"/>
+      <c r="P118" s="21"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
@@ -14989,8 +15061,8 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="O119" s="4"/>
-      <c r="P119" s="4"/>
+      <c r="O119" s="30"/>
+      <c r="P119" s="21"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
@@ -15036,8 +15108,8 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
+      <c r="O120" s="30"/>
+      <c r="P120" s="21"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
@@ -15083,8 +15155,8 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
+      <c r="O121" s="30"/>
+      <c r="P121" s="21"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
@@ -15130,8 +15202,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
+      <c r="O122" s="30"/>
+      <c r="P122" s="21"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
@@ -15177,8 +15249,8 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="O123" s="4"/>
-      <c r="P123" s="4"/>
+      <c r="O123" s="30"/>
+      <c r="P123" s="21"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
@@ -15224,8 +15296,8 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O124" s="4"/>
-      <c r="P124" s="4"/>
+      <c r="O124" s="30"/>
+      <c r="P124" s="21"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
@@ -15271,8 +15343,8 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O125" s="4"/>
-      <c r="P125" s="4"/>
+      <c r="O125" s="30"/>
+      <c r="P125" s="21"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
@@ -15318,8 +15390,8 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
+      <c r="O126" s="30"/>
+      <c r="P126" s="21"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
@@ -15365,8 +15437,8 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="O127" s="4"/>
-      <c r="P127" s="4"/>
+      <c r="O127" s="30"/>
+      <c r="P127" s="21"/>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
@@ -15412,8 +15484,8 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="O128" s="4"/>
-      <c r="P128" s="4"/>
+      <c r="O128" s="30"/>
+      <c r="P128" s="21"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
@@ -15459,8 +15531,8 @@
         <f t="shared" si="1"/>
         <v>-19</v>
       </c>
-      <c r="O129" s="4"/>
-      <c r="P129" s="4"/>
+      <c r="O129" s="30"/>
+      <c r="P129" s="21"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
@@ -15506,8 +15578,8 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="O130" s="4"/>
-      <c r="P130" s="4"/>
+      <c r="O130" s="30"/>
+      <c r="P130" s="21"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
@@ -15553,8 +15625,8 @@
         <f t="shared" ref="N131:N174" si="2">M131-L131</f>
         <v>7</v>
       </c>
-      <c r="O131" s="4"/>
-      <c r="P131" s="4"/>
+      <c r="O131" s="30"/>
+      <c r="P131" s="21"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
@@ -15600,8 +15672,8 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O132" s="4"/>
-      <c r="P132" s="4"/>
+      <c r="O132" s="30"/>
+      <c r="P132" s="21"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
@@ -15647,8 +15719,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O133" s="4"/>
-      <c r="P133" s="4"/>
+      <c r="O133" s="30"/>
+      <c r="P133" s="21"/>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
@@ -15694,8 +15766,8 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="O134" s="4"/>
-      <c r="P134" s="4"/>
+      <c r="O134" s="30"/>
+      <c r="P134" s="21"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
@@ -15741,8 +15813,8 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="O135" s="4"/>
-      <c r="P135" s="4"/>
+      <c r="O135" s="30"/>
+      <c r="P135" s="21"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
@@ -15788,8 +15860,8 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="O136" s="4"/>
-      <c r="P136" s="4"/>
+      <c r="O136" s="30"/>
+      <c r="P136" s="21"/>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
@@ -15835,8 +15907,8 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="O137" s="4"/>
-      <c r="P137" s="4"/>
+      <c r="O137" s="30"/>
+      <c r="P137" s="21"/>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
@@ -15882,8 +15954,8 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="O138" s="4"/>
-      <c r="P138" s="4"/>
+      <c r="O138" s="30"/>
+      <c r="P138" s="21"/>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
@@ -15929,8 +16001,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
+      <c r="O139" s="30"/>
+      <c r="P139" s="21"/>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
@@ -15976,8 +16048,8 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
+      <c r="O140" s="30"/>
+      <c r="P140" s="21"/>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="10" t="s">
@@ -16023,8 +16095,8 @@
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="O141" s="4"/>
-      <c r="P141" s="4"/>
+      <c r="O141" s="30"/>
+      <c r="P141" s="21"/>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="10" t="s">
@@ -16070,8 +16142,8 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="O142" s="4"/>
-      <c r="P142" s="4"/>
+      <c r="O142" s="30"/>
+      <c r="P142" s="21"/>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="10" t="s">
@@ -16117,8 +16189,8 @@
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="O143" s="4"/>
-      <c r="P143" s="4"/>
+      <c r="O143" s="30"/>
+      <c r="P143" s="21"/>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="10" t="s">
@@ -16164,8 +16236,8 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="O144" s="4"/>
-      <c r="P144" s="4"/>
+      <c r="O144" s="30"/>
+      <c r="P144" s="21"/>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="10" t="s">
@@ -16211,8 +16283,8 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="O145" s="4"/>
-      <c r="P145" s="4"/>
+      <c r="O145" s="30"/>
+      <c r="P145" s="21"/>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="10" t="s">
@@ -16258,8 +16330,8 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="O146" s="4"/>
-      <c r="P146" s="4"/>
+      <c r="O146" s="30"/>
+      <c r="P146" s="21"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="10" t="s">
@@ -16305,8 +16377,8 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="O147" s="4"/>
-      <c r="P147" s="4"/>
+      <c r="O147" s="30"/>
+      <c r="P147" s="21"/>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
@@ -16352,8 +16424,8 @@
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="O148" s="4"/>
-      <c r="P148" s="4"/>
+      <c r="O148" s="30"/>
+      <c r="P148" s="21"/>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="10" t="s">
@@ -16399,8 +16471,8 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="O149" s="4"/>
-      <c r="P149" s="4"/>
+      <c r="O149" s="30"/>
+      <c r="P149" s="21"/>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="10" t="s">
@@ -16446,8 +16518,8 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="O150" s="4"/>
-      <c r="P150" s="4"/>
+      <c r="O150" s="30"/>
+      <c r="P150" s="21"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="10" t="s">
@@ -16493,8 +16565,8 @@
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="O151" s="4"/>
-      <c r="P151" s="4"/>
+      <c r="O151" s="30"/>
+      <c r="P151" s="21"/>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="10" t="s">
@@ -16540,8 +16612,8 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="O152" s="4"/>
-      <c r="P152" s="4"/>
+      <c r="O152" s="30"/>
+      <c r="P152" s="21"/>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="10" t="s">
@@ -16587,8 +16659,8 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="O153" s="4"/>
-      <c r="P153" s="4"/>
+      <c r="O153" s="30"/>
+      <c r="P153" s="21"/>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="10" t="s">
@@ -16634,8 +16706,8 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="O154" s="4"/>
-      <c r="P154" s="4"/>
+      <c r="O154" s="30"/>
+      <c r="P154" s="21"/>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="10" t="s">
@@ -16681,8 +16753,8 @@
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
-      <c r="O155" s="4"/>
-      <c r="P155" s="4"/>
+      <c r="O155" s="30"/>
+      <c r="P155" s="21"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="10" t="s">
@@ -16728,8 +16800,8 @@
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="O156" s="4"/>
-      <c r="P156" s="4"/>
+      <c r="O156" s="30"/>
+      <c r="P156" s="21"/>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="10" t="s">
@@ -16775,8 +16847,8 @@
         <f t="shared" si="2"/>
         <v>272</v>
       </c>
-      <c r="O157" s="4"/>
-      <c r="P157" s="4"/>
+      <c r="O157" s="30"/>
+      <c r="P157" s="21"/>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="10" t="s">
@@ -16822,8 +16894,8 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="O158" s="4"/>
-      <c r="P158" s="4"/>
+      <c r="O158" s="30"/>
+      <c r="P158" s="21"/>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="10" t="s">
@@ -16869,8 +16941,8 @@
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="O159" s="4"/>
-      <c r="P159" s="4"/>
+      <c r="O159" s="30"/>
+      <c r="P159" s="21"/>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="10" t="s">
@@ -16916,8 +16988,8 @@
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
-      <c r="O160" s="4"/>
-      <c r="P160" s="4"/>
+      <c r="O160" s="30"/>
+      <c r="P160" s="21"/>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="10" t="s">
@@ -16963,8 +17035,8 @@
         <f t="shared" si="2"/>
         <v>113</v>
       </c>
-      <c r="O161" s="4"/>
-      <c r="P161" s="4"/>
+      <c r="O161" s="30"/>
+      <c r="P161" s="21"/>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="10" t="s">
@@ -17010,8 +17082,8 @@
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="O162" s="4"/>
-      <c r="P162" s="4"/>
+      <c r="O162" s="30"/>
+      <c r="P162" s="21"/>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="10" t="s">
@@ -17057,8 +17129,8 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="O163" s="4"/>
-      <c r="P163" s="4"/>
+      <c r="O163" s="30"/>
+      <c r="P163" s="21"/>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="10" t="s">
@@ -17104,8 +17176,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O164" s="4"/>
-      <c r="P164" s="4"/>
+      <c r="O164" s="30"/>
+      <c r="P164" s="21"/>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="10" t="s">
@@ -17151,8 +17223,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O165" s="4"/>
-      <c r="P165" s="4"/>
+      <c r="O165" s="30"/>
+      <c r="P165" s="21"/>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="10" t="s">
@@ -17198,8 +17270,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O166" s="4"/>
-      <c r="P166" s="4"/>
+      <c r="O166" s="30"/>
+      <c r="P166" s="21"/>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="10" t="s">
@@ -17245,8 +17317,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O167" s="4"/>
-      <c r="P167" s="4"/>
+      <c r="O167" s="30"/>
+      <c r="P167" s="21"/>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="10" t="s">
@@ -17292,8 +17364,8 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="O168" s="4"/>
-      <c r="P168" s="4"/>
+      <c r="O168" s="30"/>
+      <c r="P168" s="21"/>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="10" t="s">
@@ -17339,8 +17411,8 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="O169" s="4"/>
-      <c r="P169" s="4"/>
+      <c r="O169" s="30"/>
+      <c r="P169" s="21"/>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="10" t="s">
@@ -17386,8 +17458,8 @@
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="O170" s="4"/>
-      <c r="P170" s="4"/>
+      <c r="O170" s="30"/>
+      <c r="P170" s="21"/>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="10" t="s">
@@ -17433,8 +17505,8 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="O171" s="4"/>
-      <c r="P171" s="4"/>
+      <c r="O171" s="30"/>
+      <c r="P171" s="21"/>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="10" t="s">
@@ -17480,8 +17552,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O172" s="4"/>
-      <c r="P172" s="4"/>
+      <c r="O172" s="30"/>
+      <c r="P172" s="21"/>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="10" t="s">
@@ -17527,8 +17599,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O173" s="4"/>
-      <c r="P173" s="4"/>
+      <c r="O173" s="30"/>
+      <c r="P173" s="21"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="10" t="s">
@@ -17574,8 +17646,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O174" s="4"/>
-      <c r="P174" s="4"/>
+      <c r="O174" s="30"/>
+      <c r="P174" s="21"/>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="10" t="s">
@@ -17620,10 +17692,14 @@
       <c r="N175" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="O175" s="4"/>
-      <c r="P175" s="4"/>
+      <c r="O175" s="31"/>
+      <c r="P175" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="P2:P175"/>
+    <mergeCell ref="O2:O175"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>